<commit_message>
mega commit (bad practice)
</commit_message>
<xml_diff>
--- a/gse/configs/CMS_Avionics_Channels.xlsx
+++ b/gse/configs/CMS_Avionics_Channels.xlsx
@@ -300,10 +300,10 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.11"/>
@@ -696,10 +696,10 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.95"/>
   </cols>
@@ -1047,7 +1047,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
lotta changes, sept 27
</commit_message>
<xml_diff>
--- a/gse/configs/CMS_Avionics_Channels.xlsx
+++ b/gse/configs/CMS_Avionics_Channels.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -90,88 +90,100 @@
     <t xml:space="preserve">FU_UPPER_REDLINE</t>
   </si>
   <si>
+    <t xml:space="preserve">FU_UPPER_REDLINE_HIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OX_UPPER_REDLINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OX_UPPER_REDLINE_HIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FREE_SPACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random_ass_adc_channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI_TEMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num Args</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibration Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_FU_UPPER_SETP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_FU_LOWER_SETP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_OX_UPPER_SETP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_OX_LOWER_SETP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_FU_STATE_REGULATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_FU_STATE_ISOLATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_FU_STATE_OPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_OX_STATE_REGULATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_OX_STATE_ISOLATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_OX_STATE_OPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_BB_STATE_REGULATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_BB_STATE_ISOLATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_BB_STATE_OPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_FU_UPPER_REDLINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_FU_LOWER_REDLINE</t>
+  </si>
+  <si>
     <t xml:space="preserve">FU_LOWER_REDLINE</t>
   </si>
   <si>
-    <t xml:space="preserve">OX_UPPER_REDLINE</t>
+    <t xml:space="preserve">SET_OX_UPPER_REDLINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_OX_LOWER_REDLINE</t>
   </si>
   <si>
     <t xml:space="preserve">OX_LOWER_REDLINE</t>
   </si>
   <si>
-    <t xml:space="preserve">FREE_SPACE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">u64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">random_ass_adc_channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Num Args</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calibration Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_FU_UPPER_SETP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_FU_LOWER_SETP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_OX_UPPER_SETP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_OX_LOWER_SETP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_FU_STATE_REGULATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_FU_STATE_ISOLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_FU_STATE_OPEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_OX_STATE_REGULATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_OX_STATE_ISOLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_OX_STATE_OPEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_BB_STATE_REGULATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_BB_STATE_ISOLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_BB_STATE_OPEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">START</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_FU_UPPER_REDLINE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_FU_LOWER_REDLINE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_OX_UPPER_REDLINE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET_OX_LOWER_REDLINE</t>
+    <t xml:space="preserve">REDLINE_RESET</t>
   </si>
   <si>
     <t xml:space="preserve">ADC Voltage</t>
@@ -297,13 +309,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.11"/>
@@ -347,7 +359,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>-33.59883</v>
+        <v>-21.4589241880161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,7 +381,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>-30.79381</v>
+        <v>-19.2575866037113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,8 +392,8 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="n">
-        <f aca="false">499.706495 * 5</f>
-        <v>2498.532475</v>
+        <f aca="false">499.706495*3 - 45</f>
+        <v>1454.119485</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>-3.510611027</v>
@@ -390,7 +402,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>-165.2682</v>
+        <v>-99.4067279203838</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,6 +421,9 @@
       <c r="E5" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -426,6 +441,9 @@
       <c r="E6" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -437,6 +455,9 @@
       <c r="E7" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -448,6 +469,9 @@
       <c r="E8" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -459,6 +483,9 @@
       <c r="E9" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -470,6 +497,9 @@
       <c r="E10" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -491,7 +521,7 @@
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">$F$3</f>
-        <v>-30.79381</v>
+        <v>-19.2575866037113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,7 +544,7 @@
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">$F$3</f>
-        <v>-30.79381</v>
+        <v>-19.2575866037113</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,7 +567,7 @@
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">$F$2</f>
-        <v>-33.59883</v>
+        <v>-21.4589241880161</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,7 +590,7 @@
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">$F$2</f>
-        <v>-33.59883</v>
+        <v>-21.4589241880161</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,7 +613,7 @@
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">$F$3</f>
-        <v>-30.79381</v>
+        <v>-19.2575866037113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,20 +623,11 @@
       <c r="B16" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C16" s="0" t="n">
-        <f aca="false">$C$3</f>
-        <v>300.0360531</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <f aca="false">$D$3</f>
-        <v>0.074545204</v>
-      </c>
       <c r="E16" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F16" s="0" t="n">
-        <f aca="false">$F$3</f>
-        <v>-30.79381</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,7 +650,7 @@
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">$F$2</f>
-        <v>-33.59883</v>
+        <v>-21.4589241880161</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,20 +660,11 @@
       <c r="B18" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="C18" s="0" t="n">
-        <f aca="false">$C$2</f>
-        <v>300.0279615</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <f aca="false">$D$2</f>
-        <v>0.373452149</v>
-      </c>
       <c r="E18" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F18" s="0" t="n">
-        <f aca="false">$F$2</f>
-        <v>-33.59883</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,10 +672,13 @@
         <v>25</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>26</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -673,8 +688,38 @@
       <c r="B20" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="E20" s="0" t="s">
         <v>26</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">1/1000</f>
+        <v>0.001</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -693,13 +738,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.95"/>
   </cols>
@@ -715,15 +760,15 @@
         <v>4</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -740,7 +785,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -757,7 +802,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -774,7 +819,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -791,7 +836,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -805,7 +850,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -819,7 +864,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -833,7 +878,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -847,7 +892,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>8</v>
@@ -861,7 +906,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>9</v>
@@ -875,7 +920,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>10</v>
@@ -889,7 +934,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>11</v>
@@ -903,7 +948,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>12</v>
@@ -917,7 +962,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>13</v>
@@ -931,7 +976,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>14</v>
@@ -945,7 +990,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>15</v>
@@ -959,7 +1004,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>16</v>
@@ -976,7 +1021,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>17</v>
@@ -988,12 +1033,12 @@
         <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>18</v>
@@ -1010,7 +1055,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>19</v>
@@ -1022,7 +1067,21 @@
         <v>1</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>24</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1043,23 +1102,23 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,10 +1219,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
naming updates for synnax 0.49
</commit_message>
<xml_diff>
--- a/gse/configs/CMS_Avionics_Channels.xlsx
+++ b/gse/configs/CMS_Avionics_Channels.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="telem_channels" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="command_channels" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="calibration" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="telem_channels" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="command_channels" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="calibration" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -42,37 +42,37 @@
     <t xml:space="preserve">Zeroing Offset</t>
   </si>
   <si>
-    <t xml:space="preserve">PT-OX-201</t>
+    <t xml:space="preserve">PT_OX_201</t>
   </si>
   <si>
     <t xml:space="preserve">f64</t>
   </si>
   <si>
-    <t xml:space="preserve">PT-FU-201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT-HE-201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SV-HE-201-state</t>
+    <t xml:space="preserve">PT_FU_201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT_HE_201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SV_HE_201_state</t>
   </si>
   <si>
     <t xml:space="preserve">u8</t>
   </si>
   <si>
-    <t xml:space="preserve">SV-HE-202-state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SV-HE-201-position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SV-HE-202-position</t>
+    <t xml:space="preserve">SV_HE_202_state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SV_HE_201_position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SV_HE_202_position</t>
   </si>
   <si>
     <t xml:space="preserve">FU_UPPER_SETP</t>
@@ -205,10 +205,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -275,20 +274,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,421 +307,527 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <f aca="false">100.0093205 * 3</f>
         <v>300.0279615</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>0.373452149</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>-21.4589241880161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <f aca="false">100.0120177 * 3</f>
         <v>300.0360531</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <f aca="false">0.074545204</f>
         <v>0.074545204</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="n">
         <v>-19.2575866037113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <f aca="false">499.706495*3 - 45</f>
         <v>1454.119485</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="2" t="n">
         <v>-3.510611027</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <v>-99.4067279203838</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="n">
+      <c r="B5" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>-250</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>-250</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="0" t="n">
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="0" t="n">
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="0" t="n">
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="0" t="n">
+      <c r="B9" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="0" t="n">
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <f aca="false">$C$3</f>
         <v>300.0360531</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <f aca="false">$D$3</f>
         <v>0.074545204</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="0" t="n">
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="n">
         <f aca="false">$F$3</f>
         <v>-19.2575866037113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <f aca="false">$C$3</f>
         <v>300.0360531</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <f aca="false">$D$3</f>
         <v>0.074545204</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="0" t="n">
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="n">
         <f aca="false">$F$3</f>
         <v>-19.2575866037113</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <f aca="false">$C$2</f>
         <v>300.0279615</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <f aca="false">$D$2</f>
         <v>0.373452149</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="0" t="n">
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="n">
         <f aca="false">$F$2</f>
         <v>-21.4589241880161</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <f aca="false">$C$2</f>
         <v>300.0279615</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <f aca="false">$D$2</f>
         <v>0.373452149</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="0" t="n">
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="n">
         <f aca="false">$F$2</f>
         <v>-21.4589241880161</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <f aca="false">$C$3</f>
         <v>300.0360531</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <f aca="false">$D$3</f>
         <v>0.074545204</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="0" t="n">
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="n">
         <f aca="false">$F$3</f>
         <v>-19.2575866037113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="0" t="n">
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <f aca="false">$C$2</f>
         <v>300.0279615</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <f aca="false">$D$2</f>
         <v>0.373452149</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="0" t="n">
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="n">
         <f aca="false">$F$2</f>
         <v>-21.4589241880161</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="0" t="n">
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="D20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <f aca="false">1/1000</f>
         <v>0.001</v>
       </c>
-      <c r="D21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="0" t="n">
+      <c r="D21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -734,7 +843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -744,343 +853,343 @@
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="0" t="n">
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="0" t="n">
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="0" t="n">
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="0" t="n">
+      <c r="B9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="0" t="n">
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="0" t="n">
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="0" t="n">
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="0" t="n">
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="0" t="n">
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="0" t="n">
+      <c r="B15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="0" t="n">
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="0" t="n">
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="0" t="n">
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="0" t="n">
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="0" t="n">
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="0" t="n">
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="0" t="n">
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1096,7 +1205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1106,130 +1215,130 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>0.101</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>48564203.3003731</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>0.11</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>52453767.7437909</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>56676330.8190299</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>0.131</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>61340637.5350734</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>0.141</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>65564288.9552239</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>0.151</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>69742511.4360313</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="A9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>5839384.78859858</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>430235385.290625</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>855165502.287709</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>1279398982.66176</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>1703360458.86034</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>2125931587.72087</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="4" t="n">
         <v>2.35714724017E-009</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>-0.013901338240206</v>
       </c>
     </row>

</xml_diff>